<commit_message>
divers scripts pour mettre à jou elo
</commit_message>
<xml_diff>
--- a/backend/Elo_Man.xlsx
+++ b/backend/Elo_Man.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Developpement\Claude\tennis-pronostics\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF7BBB-A0CA-412C-852D-84348CB8605A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE613551-D564-4F75-83C2-8EA9D6C3315B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADCCBAAC-95CD-485B-926F-A1D479F80639}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Tommy Paul</t>
   </si>
   <si>
-    <t>Taylor Fritz</t>
-  </si>
-  <si>
     <t>Daniil Medvedev</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Mariano Navone</t>
   </si>
   <si>
-    <t>Jaume Munar</t>
-  </si>
-  <si>
     <t>Miomir Kecmanovic</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>Yoshihito Nishioka</t>
   </si>
   <si>
-    <t>Jason Kubler</t>
-  </si>
-  <si>
     <t>Roman Safiullin</t>
   </si>
   <si>
@@ -296,9 +287,6 @@
     <t>Zhizhen Zhang</t>
   </si>
   <si>
-    <t>Pablo Carreno Busta</t>
-  </si>
-  <si>
     <t>Luciano Darderi</t>
   </si>
   <si>
@@ -320,9 +308,6 @@
     <t>Raphael Collignon</t>
   </si>
   <si>
-    <t>Jan Lennard Struff</t>
-  </si>
-  <si>
     <t>Nicolas Jarry</t>
   </si>
   <si>
@@ -353,9 +338,6 @@
     <t>Stan Wawrinka</t>
   </si>
   <si>
-    <t>Christopher Oconnell</t>
-  </si>
-  <si>
     <t>Dusan Lajovic</t>
   </si>
   <si>
@@ -389,9 +371,6 @@
     <t>Rinky Hijikata</t>
   </si>
   <si>
-    <t>Pedro Martinez</t>
-  </si>
-  <si>
     <t>Hugo Dellien</t>
   </si>
   <si>
@@ -458,9 +437,6 @@
     <t>Nicolas Moreno De Alboran</t>
   </si>
   <si>
-    <t>Pierre Hugues Herbert</t>
-  </si>
-  <si>
     <t>Roman Andres Burruchaga</t>
   </si>
   <si>
@@ -527,9 +503,6 @@
     <t>Hyeon Chung</t>
   </si>
   <si>
-    <t>Marc Andrea Huesler</t>
-  </si>
-  <si>
     <t>Luca Van Assche</t>
   </si>
   <si>
@@ -572,9 +545,6 @@
     <t>James Duckworth</t>
   </si>
   <si>
-    <t>Thiago Monteiro</t>
-  </si>
-  <si>
     <t>Mattia Bellucci</t>
   </si>
   <si>
@@ -602,9 +572,6 @@
     <t>Harold Mayot</t>
   </si>
   <si>
-    <t>J J Wolf</t>
-  </si>
-  <si>
     <t>Lukas Klein</t>
   </si>
   <si>
@@ -623,9 +590,6 @@
     <t>Tristan Boyer</t>
   </si>
   <si>
-    <t>Albert Ramos</t>
-  </si>
-  <si>
     <t>Constant Lestienne</t>
   </si>
   <si>
@@ -641,9 +605,6 @@
     <t>Benjamin Hassan</t>
   </si>
   <si>
-    <t>Seong Chan Hong</t>
-  </si>
-  <si>
     <t>Mikhail Kukushkin</t>
   </si>
   <si>
@@ -677,9 +638,6 @@
     <t>Alexander Ritschard</t>
   </si>
   <si>
-    <t>James Trotter</t>
-  </si>
-  <si>
     <t>Alex Barrena</t>
   </si>
   <si>
@@ -773,9 +731,6 @@
     <t>Clement Tabur</t>
   </si>
   <si>
-    <t>Coleman Wong</t>
-  </si>
-  <si>
     <t>Juan Pablo Varillas</t>
   </si>
   <si>
@@ -971,9 +926,6 @@
     <t>Egor Gerasimov</t>
   </si>
   <si>
-    <t>Tung Lin Wu</t>
-  </si>
-  <si>
     <t>Nicolai Budkov Kjaer</t>
   </si>
   <si>
@@ -992,9 +944,6 @@
     <t>Lautaro Midon</t>
   </si>
   <si>
-    <t>Inaki Montes De La Torre</t>
-  </si>
-  <si>
     <t>Johannus Monday</t>
   </si>
   <si>
@@ -1028,9 +977,6 @@
     <t>Oliver Crawford</t>
   </si>
   <si>
-    <t>Santiago Fa Rodriguez Taverna</t>
-  </si>
-  <si>
     <t>Filip Cristian Jianu</t>
   </si>
   <si>
@@ -1130,9 +1076,6 @@
     <t>Maximus Jones</t>
   </si>
   <si>
-    <t>Murkel Alejandro Dellien Velasco</t>
-  </si>
-  <si>
     <t>Alex Martinez</t>
   </si>
   <si>
@@ -1181,9 +1124,6 @@
     <t>Nicolas Kicker</t>
   </si>
   <si>
-    <t>Antoine Cornut Chauvinc</t>
-  </si>
-  <si>
     <t>Abedallah Shelbayh</t>
   </si>
   <si>
@@ -1283,9 +1223,6 @@
     <t>Tristan Lamasine</t>
   </si>
   <si>
-    <t>Sasi Kumar Mukund</t>
-  </si>
-  <si>
     <t>Evgeny Karlovskiy</t>
   </si>
   <si>
@@ -1307,9 +1244,6 @@
     <t>Martin Krumich</t>
   </si>
   <si>
-    <t>Nikolas Sanchez Izquierdo</t>
-  </si>
-  <si>
     <t>Govind Nanda</t>
   </si>
   <si>
@@ -1346,9 +1280,6 @@
     <t>Renzo Olivo</t>
   </si>
   <si>
-    <t>Diego Dedura Palomero</t>
-  </si>
-  <si>
     <t>Lucas Poullain</t>
   </si>
   <si>
@@ -1421,9 +1352,6 @@
     <t>Mateus Alves</t>
   </si>
   <si>
-    <t>Roberto Cid</t>
-  </si>
-  <si>
     <t>Naoki Nakagawa</t>
   </si>
   <si>
@@ -1445,9 +1373,6 @@
     <t>Pedro Araujo</t>
   </si>
   <si>
-    <t>Juan Alejandro Hernandez Serrano</t>
-  </si>
-  <si>
     <t>Valerio Aboian</t>
   </si>
   <si>
@@ -1487,9 +1412,6 @@
     <t>Andrea Picchione</t>
   </si>
   <si>
-    <t>Juan Carlos Aguilar</t>
-  </si>
-  <si>
     <t>Alexis Gautier</t>
   </si>
   <si>
@@ -1515,6 +1437,84 @@
   </si>
   <si>
     <t>hardElo</t>
+  </si>
+  <si>
+    <t>Taylor Harry Fritz</t>
+  </si>
+  <si>
+    <t>Jaume Antoni Munar Clar</t>
+  </si>
+  <si>
+    <t>Jason Murray Kubler</t>
+  </si>
+  <si>
+    <t>Pablo Carreno-Busta</t>
+  </si>
+  <si>
+    <t>Jan-Lennard Struff</t>
+  </si>
+  <si>
+    <t>Christopher O'Connell</t>
+  </si>
+  <si>
+    <t>Pedro Martinez Portero</t>
+  </si>
+  <si>
+    <t>Pierre-Hugues Herbert</t>
+  </si>
+  <si>
+    <t>Marc-Andrea Huesler</t>
+  </si>
+  <si>
+    <t>Thiago Moura Monteiro</t>
+  </si>
+  <si>
+    <t>Jeff Wolf</t>
+  </si>
+  <si>
+    <t>Albert Ramos-Vinolas</t>
+  </si>
+  <si>
+    <t>Seongchan Hong</t>
+  </si>
+  <si>
+    <t>James Kent Trotter</t>
+  </si>
+  <si>
+    <t>Chak Lam Coleman Wong</t>
+  </si>
+  <si>
+    <t>Tung-Lin Wu</t>
+  </si>
+  <si>
+    <t>Inaki Montes-De La Torre</t>
+  </si>
+  <si>
+    <t>Santiago Rodriguez Taverna</t>
+  </si>
+  <si>
+    <t>Murkel Dellien</t>
+  </si>
+  <si>
+    <t>Antoine Cornut-Chauvinc</t>
+  </si>
+  <si>
+    <t>Mukund Sasikumar</t>
+  </si>
+  <si>
+    <t>Nikolas Sanchez-Izquierdo</t>
+  </si>
+  <si>
+    <t>Diego Dedura-Palomero</t>
+  </si>
+  <si>
+    <t>Roberto Cid Subervi</t>
+  </si>
+  <si>
+    <t>Juan Alejandro Hernandez</t>
+  </si>
+  <si>
+    <t>Juan Carlos Manuel Aguilar</t>
   </si>
 </sst>
 </file>
@@ -1934,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959CD3DD-99C1-4727-BB03-D615B5FF12D3}">
   <dimension ref="A1:F488"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <selection activeCell="D461" sqref="D461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -1952,16 +1952,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>490</v>
+        <v>464</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>467</v>
       </c>
       <c r="B9" s="4">
         <v>1992.3</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
         <v>1989.1</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
         <v>1988.6</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4">
         <v>1983</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4">
         <v>1971.5</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4">
         <v>1962.7</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4">
         <v>1955.5</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4">
         <v>1954.1</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4">
         <v>1952.2</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
         <v>1945.8</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
         <v>1933.3</v>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
         <v>1917.8</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4">
         <v>1914.6</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="4">
         <v>1913.3</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4">
         <v>1905.9</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4">
         <v>1902.2</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4">
         <v>1899.9</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4">
         <v>1898.1</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4">
         <v>1896</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4">
         <v>1891.3</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4">
         <v>1889.8</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4">
         <v>1883.8</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4">
         <v>1878</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4">
         <v>1877.7</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4">
         <v>1876.7</v>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4">
         <v>1872.6</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4">
         <v>1867.4</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4">
         <v>1857</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="4">
         <v>1847.2</v>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="4">
         <v>1846.3</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4">
         <v>1844.4</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="4">
         <v>1844</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4">
         <v>1839.6</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4">
         <v>1834.3</v>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4">
         <v>1830.4</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4">
         <v>1827.8</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="4">
         <v>1827.8</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="4">
         <v>1824.9</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="4">
         <v>1824.3</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="4">
         <v>1810.6</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="4">
         <v>1806.4</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4">
         <v>1800.9</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="4">
         <v>1798.2</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="4">
         <v>1793.8</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="4">
         <v>1790.9</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4">
         <v>1790.3</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="4">
         <v>1790.3</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4">
         <v>1788.6</v>
@@ -3066,7 +3066,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="4">
         <v>1785.9</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="4">
         <v>1782.6</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="4">
         <v>1782.1</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4">
         <v>1781.5</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4">
         <v>1777.2</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="4">
         <v>1777</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="4">
         <v>1775.2</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="4">
         <v>1774.7</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="4">
         <v>1774</v>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="4">
         <v>1769</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>67</v>
+        <v>468</v>
       </c>
       <c r="B67" s="4">
         <v>1768.6</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B68" s="4">
         <v>1767.1</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B69" s="4">
         <v>1764.9</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" s="4">
         <v>1764.3</v>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B71" s="4">
         <v>1763</v>
@@ -3366,7 +3366,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="4">
         <v>1758.9</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B73" s="4">
         <v>1755.6</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B74" s="4">
         <v>1755</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B75" s="4">
         <v>1754.7</v>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B76" s="4">
         <v>1747.2</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B77" s="4">
         <v>1744.2</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>78</v>
+        <v>469</v>
       </c>
       <c r="B78" s="4">
         <v>1742.6</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B79" s="4">
         <v>1738.2</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B80" s="4">
         <v>1736.4</v>
@@ -3546,7 +3546,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B81" s="4">
         <v>1733.5</v>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B82" s="4">
         <v>1730.2</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B83" s="4">
         <v>1729.9</v>
@@ -3606,7 +3606,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B84" s="4">
         <v>1729.6</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B85" s="4">
         <v>1727.2</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>86</v>
+        <v>470</v>
       </c>
       <c r="B86" s="4">
         <v>1726.6</v>
@@ -3666,7 +3666,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B87" s="4">
         <v>1725.9</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B88" s="4">
         <v>1725.7</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B89" s="4">
         <v>1723.2</v>
@@ -3726,7 +3726,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B90" s="4">
         <v>1722.4</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B91" s="4">
         <v>1719.9</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B92" s="4">
         <v>1719.7</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B93" s="4">
         <v>1718.8</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>94</v>
+        <v>471</v>
       </c>
       <c r="B94" s="4">
         <v>1715.8</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B95" s="4">
         <v>1715.7</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B96" s="4">
         <v>1715.6</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B97" s="4">
         <v>1713.4</v>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B98" s="4">
         <v>1713.4</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B99" s="4">
         <v>1710.1</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B100" s="4">
         <v>1708.3</v>
@@ -3946,7 +3946,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B101" s="4">
         <v>1706.4</v>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B102" s="4">
         <v>1705</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B103" s="4">
         <v>1702.6</v>
@@ -4006,7 +4006,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B104" s="4">
         <v>1700.3</v>
@@ -4026,7 +4026,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>105</v>
+        <v>472</v>
       </c>
       <c r="B105" s="4">
         <v>1699.3</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B106" s="4">
         <v>1693</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B107" s="4">
         <v>1692.5</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B108" s="4">
         <v>1685.8</v>
@@ -4106,7 +4106,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B109" s="4">
         <v>1684.8</v>
@@ -4126,7 +4126,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B110" s="4">
         <v>1684.8</v>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B111" s="4">
         <v>1682.7</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B112" s="4">
         <v>1681.5</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B113" s="4">
         <v>1681.4</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B114" s="4">
         <v>1680.1</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B115" s="4">
         <v>1679.8</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B116" s="4">
         <v>1677.4</v>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>117</v>
+        <v>473</v>
       </c>
       <c r="B117" s="4">
         <v>1672.3</v>
@@ -4286,7 +4286,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B118" s="4">
         <v>1670.9</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B119" s="4">
         <v>1669.5</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B120" s="4">
         <v>1669.2</v>
@@ -4346,7 +4346,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B121" s="4">
         <v>1667.3</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B122" s="4">
         <v>1665.5</v>
@@ -4386,7 +4386,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B123" s="4">
         <v>1664.9</v>
@@ -4406,7 +4406,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B124" s="4">
         <v>1664</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B125" s="4">
         <v>1663</v>
@@ -4446,7 +4446,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B126" s="4">
         <v>1660.7</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B127" s="4">
         <v>1659.8</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B128" s="4">
         <v>1659.2</v>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B129" s="4">
         <v>1657.3</v>
@@ -4526,7 +4526,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B130" s="4">
         <v>1657.2</v>
@@ -4546,7 +4546,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B131" s="4">
         <v>1657.1</v>
@@ -4566,7 +4566,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B132" s="4">
         <v>1656.3</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B133" s="4">
         <v>1655.3</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B134" s="4">
         <v>1655.3</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B135" s="4">
         <v>1654</v>
@@ -4646,7 +4646,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B136" s="4">
         <v>1653.1</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B137" s="4">
         <v>1650.3</v>
@@ -4686,7 +4686,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B138" s="4">
         <v>1648.8</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B139" s="4">
         <v>1648.5</v>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>140</v>
+        <v>474</v>
       </c>
       <c r="B140" s="4">
         <v>1647.7</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B141" s="4">
         <v>1647.5</v>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B142" s="4">
         <v>1646.3</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B143" s="4">
         <v>1645.9</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B144" s="4">
         <v>1642.7</v>
@@ -4826,7 +4826,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B145" s="4">
         <v>1640.6</v>
@@ -4846,7 +4846,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B146" s="4">
         <v>1639.8</v>
@@ -4866,7 +4866,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B147" s="4">
         <v>1637.8</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B148" s="4">
         <v>1635.7</v>
@@ -4906,7 +4906,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B149" s="4">
         <v>1634.6</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B150" s="4">
         <v>1632.8</v>
@@ -4946,7 +4946,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B151" s="4">
         <v>1632.7</v>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B152" s="4">
         <v>1632.5</v>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B153" s="4">
         <v>1631.8</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B154" s="4">
         <v>1631.7</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B155" s="4">
         <v>1629.9</v>
@@ -5046,7 +5046,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B156" s="4">
         <v>1629.7</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B157" s="4">
         <v>1628.2</v>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B158" s="4">
         <v>1626.5</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B159" s="4">
         <v>1625.1</v>
@@ -5126,7 +5126,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B160" s="4">
         <v>1622.6</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B161" s="4">
         <v>1622.4</v>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B162" s="4">
         <v>1621.9</v>
@@ -5186,7 +5186,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>163</v>
+        <v>475</v>
       </c>
       <c r="B163" s="4">
         <v>1619</v>
@@ -5206,7 +5206,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B164" s="4">
         <v>1617.8</v>
@@ -5226,7 +5226,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B165" s="4">
         <v>1616.8</v>
@@ -5246,7 +5246,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B166" s="4">
         <v>1615.1</v>
@@ -5266,7 +5266,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B167" s="4">
         <v>1614.6</v>
@@ -5286,7 +5286,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B168" s="4">
         <v>1609.2</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B169" s="4">
         <v>1609.1</v>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B170" s="4">
         <v>1608.7</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B171" s="4">
         <v>1608.4</v>
@@ -5366,7 +5366,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B172" s="4">
         <v>1606.5</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B173" s="4">
         <v>1604.6</v>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B174" s="4">
         <v>1604.5</v>
@@ -5426,7 +5426,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B175" s="4">
         <v>1603.9</v>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B176" s="4">
         <v>1603.7</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B177" s="4">
         <v>1602.5</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>178</v>
+        <v>476</v>
       </c>
       <c r="B178" s="4">
         <v>1600.4</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B179" s="4">
         <v>1600.2</v>
@@ -5526,7 +5526,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B180" s="4">
         <v>1598.6</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B181" s="4">
         <v>1595.6</v>
@@ -5566,7 +5566,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B182" s="4">
         <v>1595.4</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B183" s="4">
         <v>1595</v>
@@ -5606,7 +5606,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B184" s="4">
         <v>1591.9</v>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B185" s="4">
         <v>1591.4</v>
@@ -5646,7 +5646,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B186" s="4">
         <v>1586.8</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B187" s="4">
         <v>1586.7</v>
@@ -5686,7 +5686,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>188</v>
+        <v>477</v>
       </c>
       <c r="B188" s="4">
         <v>1586.4</v>
@@ -5706,7 +5706,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B189" s="4">
         <v>1585.1</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B190" s="4">
         <v>1583.4</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B191" s="4">
         <v>1582.6</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B192" s="4">
         <v>1582.6</v>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B193" s="4">
         <v>1581.7</v>
@@ -5806,7 +5806,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B194" s="4">
         <v>1581.4</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>195</v>
+        <v>478</v>
       </c>
       <c r="B195" s="4">
         <v>1576.7</v>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B196" s="4">
         <v>1575.5</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B197" s="4">
         <v>1575.3</v>
@@ -5886,7 +5886,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B198" s="4">
         <v>1574.2</v>
@@ -5906,7 +5906,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="B199" s="4">
         <v>1573.5</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B200" s="4">
         <v>1573.2</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>201</v>
+        <v>479</v>
       </c>
       <c r="B201" s="4">
         <v>1573</v>
@@ -5966,7 +5966,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B202" s="4">
         <v>1571.6</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B203" s="4">
         <v>1570.6</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B204" s="4">
         <v>1566.1</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B205" s="4">
         <v>1565.5</v>
@@ -6046,7 +6046,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B206" s="4">
         <v>1564.4</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B207" s="4">
         <v>1563.3</v>
@@ -6086,7 +6086,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B208" s="4">
         <v>1562.5</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B209" s="4">
         <v>1561.3</v>
@@ -6126,7 +6126,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B210" s="4">
         <v>1560.8</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B211" s="4">
         <v>1557</v>
@@ -6166,7 +6166,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B212" s="4">
         <v>1556.4</v>
@@ -6186,7 +6186,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>213</v>
+        <v>480</v>
       </c>
       <c r="B213" s="4">
         <v>1555.7</v>
@@ -6206,7 +6206,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B214" s="4">
         <v>1550.1</v>
@@ -6226,7 +6226,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B215" s="4">
         <v>1549.5</v>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B216" s="4">
         <v>1549.4</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B217" s="4">
         <v>1548.6</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B218" s="4">
         <v>1546.7</v>
@@ -6306,7 +6306,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B219" s="4">
         <v>1543.7</v>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B220" s="4">
         <v>1541.4</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B221" s="4">
         <v>1537.5</v>
@@ -6366,7 +6366,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B222" s="4">
         <v>1536.8</v>
@@ -6386,7 +6386,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B223" s="4">
         <v>1535.5</v>
@@ -6406,7 +6406,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B224" s="4">
         <v>1535.2</v>
@@ -6426,7 +6426,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B225" s="4">
         <v>1533.7</v>
@@ -6446,7 +6446,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B226" s="4">
         <v>1532.7</v>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B227" s="4">
         <v>1532.1</v>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B228" s="4">
         <v>1529.4</v>
@@ -6506,7 +6506,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B229" s="4">
         <v>1529.3</v>
@@ -6526,7 +6526,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B230" s="4">
         <v>1528.7</v>
@@ -6546,7 +6546,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B231" s="4">
         <v>1528.5</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B232" s="4">
         <v>1528.5</v>
@@ -6586,7 +6586,7 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B233" s="4">
         <v>1528.1</v>
@@ -6606,7 +6606,7 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B234" s="4">
         <v>1526.1</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B235" s="4">
         <v>1525.3</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B236" s="4">
         <v>1523.8</v>
@@ -6666,7 +6666,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B237" s="4">
         <v>1522.8</v>
@@ -6686,7 +6686,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B238" s="4">
         <v>1520.8</v>
@@ -6706,7 +6706,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B239" s="4">
         <v>1520.5</v>
@@ -6726,7 +6726,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B240" s="4">
         <v>1520.2</v>
@@ -6746,7 +6746,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="B241" s="4">
         <v>1520.1</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B242" s="4">
         <v>1520.1</v>
@@ -6786,7 +6786,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B243" s="4">
         <v>1519.1</v>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B244" s="4">
         <v>1518.5</v>
@@ -6826,7 +6826,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
-        <v>245</v>
+        <v>481</v>
       </c>
       <c r="B245" s="4">
         <v>1516.8</v>
@@ -6846,7 +6846,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B246" s="4">
         <v>1515.8</v>
@@ -6866,7 +6866,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B247" s="4">
         <v>1515.6</v>
@@ -6886,7 +6886,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B248" s="4">
         <v>1514.4</v>
@@ -6906,7 +6906,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B249" s="4">
         <v>1514.2</v>
@@ -6926,7 +6926,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B250" s="4">
         <v>1512.8</v>
@@ -6946,7 +6946,7 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B251" s="4">
         <v>1511.9</v>
@@ -6966,7 +6966,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B252" s="4">
         <v>1511</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B253" s="4">
         <v>1510.1</v>
@@ -7006,7 +7006,7 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="B254" s="4">
         <v>1505</v>
@@ -7026,7 +7026,7 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="B255" s="4">
         <v>1504.5</v>
@@ -7046,7 +7046,7 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B256" s="4">
         <v>1504.2</v>
@@ -7066,7 +7066,7 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B257" s="4">
         <v>1503.6</v>
@@ -7086,7 +7086,7 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B258" s="4">
         <v>1502.2</v>
@@ -7106,7 +7106,7 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B259" s="4">
         <v>1500.5</v>
@@ -7126,7 +7126,7 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B260" s="4">
         <v>1498.8</v>
@@ -7146,7 +7146,7 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="B261" s="4">
         <v>1498.2</v>
@@ -7166,7 +7166,7 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B262" s="4">
         <v>1496.1</v>
@@ -7186,7 +7186,7 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B263" s="4">
         <v>1495.3</v>
@@ -7206,7 +7206,7 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B264" s="4">
         <v>1494.6</v>
@@ -7226,7 +7226,7 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B265" s="4">
         <v>1493.8</v>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="B266" s="4">
         <v>1492.6</v>
@@ -7266,7 +7266,7 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B267" s="4">
         <v>1490.3</v>
@@ -7286,7 +7286,7 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B268" s="4">
         <v>1490</v>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B269" s="4">
         <v>1489.2</v>
@@ -7326,7 +7326,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B270" s="4">
         <v>1488.7</v>
@@ -7346,7 +7346,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B271" s="4">
         <v>1488.1</v>
@@ -7366,7 +7366,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B272" s="4">
         <v>1485.9</v>
@@ -7386,7 +7386,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B273" s="4">
         <v>1484.9</v>
@@ -7406,7 +7406,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B274" s="4">
         <v>1484.3</v>
@@ -7426,7 +7426,7 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="5" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B275" s="4">
         <v>1483.1</v>
@@ -7446,7 +7446,7 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B276" s="4">
         <v>1482.3</v>
@@ -7466,7 +7466,7 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="B277" s="4">
         <v>1480.9</v>
@@ -7486,7 +7486,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="B278" s="4">
         <v>1480.6</v>
@@ -7506,7 +7506,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B279" s="4">
         <v>1480.1</v>
@@ -7526,7 +7526,7 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="5" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="B280" s="4">
         <v>1479.3</v>
@@ -7546,7 +7546,7 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="B281" s="4">
         <v>1478.8</v>
@@ -7566,7 +7566,7 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="B282" s="4">
         <v>1478.4</v>
@@ -7586,7 +7586,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="5" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="B283" s="4">
         <v>1478.4</v>
@@ -7606,7 +7606,7 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="B284" s="4">
         <v>1478.3</v>
@@ -7626,7 +7626,7 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="B285" s="4">
         <v>1477.4</v>
@@ -7646,7 +7646,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="5" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="B286" s="4">
         <v>1476</v>
@@ -7666,7 +7666,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="B287" s="4">
         <v>1475.9</v>
@@ -7686,7 +7686,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B288" s="4">
         <v>1475.6</v>
@@ -7706,7 +7706,7 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="5" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="B289" s="4">
         <v>1475.4</v>
@@ -7726,7 +7726,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B290" s="4">
         <v>1473.2</v>
@@ -7746,7 +7746,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="5" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B291" s="4">
         <v>1473</v>
@@ -7766,7 +7766,7 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B292" s="4">
         <v>1471.6</v>
@@ -7786,7 +7786,7 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="B293" s="4">
         <v>1470.7</v>
@@ -7806,7 +7806,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B294" s="4">
         <v>1467.8</v>
@@ -7826,7 +7826,7 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="5" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B295" s="4">
         <v>1467.5</v>
@@ -7846,7 +7846,7 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B296" s="4">
         <v>1467.3</v>
@@ -7866,7 +7866,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B297" s="4">
         <v>1466.1</v>
@@ -7886,7 +7886,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B298" s="4">
         <v>1463.6</v>
@@ -7906,7 +7906,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B299" s="4">
         <v>1463.4</v>
@@ -7926,7 +7926,7 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="B300" s="4">
         <v>1462.7</v>
@@ -7946,7 +7946,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="5" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="B301" s="4">
         <v>1462.6</v>
@@ -7966,7 +7966,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="B302" s="4">
         <v>1462.6</v>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B303" s="4">
         <v>1462</v>
@@ -8006,7 +8006,7 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="B304" s="4">
         <v>1459.7</v>
@@ -8026,7 +8026,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="5" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B305" s="4">
         <v>1459.4</v>
@@ -8046,7 +8046,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="5" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="B306" s="4">
         <v>1459.3</v>
@@ -8066,7 +8066,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="5" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B307" s="4">
         <v>1459</v>
@@ -8086,7 +8086,7 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="B308" s="4">
         <v>1457.4</v>
@@ -8106,7 +8106,7 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="5" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B309" s="4">
         <v>1457.2</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="B310" s="4">
         <v>1456.7</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="5" t="s">
-        <v>311</v>
+        <v>482</v>
       </c>
       <c r="B311" s="4">
         <v>1455.2</v>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B312" s="4">
         <v>1454.6</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="B313" s="4">
         <v>1453.9</v>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="B314" s="4">
         <v>1452.2</v>
@@ -8226,7 +8226,7 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B315" s="4">
         <v>1449.9</v>
@@ -8246,7 +8246,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B316" s="4">
         <v>1449.1</v>
@@ -8266,7 +8266,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="B317" s="4">
         <v>1448.3</v>
@@ -8286,7 +8286,7 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
-        <v>318</v>
+        <v>483</v>
       </c>
       <c r="B318" s="4">
         <v>1446.6</v>
@@ -8306,7 +8306,7 @@
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="B319" s="4">
         <v>1443.5</v>
@@ -8326,7 +8326,7 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="5" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="B320" s="4">
         <v>1443.2</v>
@@ -8346,7 +8346,7 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="5" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="B321" s="4">
         <v>1443.2</v>
@@ -8366,7 +8366,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="5" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="B322" s="4">
         <v>1441.4</v>
@@ -8386,7 +8386,7 @@
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="5" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="B323" s="4">
         <v>1440.9</v>
@@ -8406,7 +8406,7 @@
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="5" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="B324" s="4">
         <v>1440.6</v>
@@ -8426,7 +8426,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="5" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="B325" s="4">
         <v>1440.5</v>
@@ -8446,7 +8446,7 @@
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="5" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="B326" s="4">
         <v>1440.2</v>
@@ -8466,7 +8466,7 @@
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="5" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="B327" s="4">
         <v>1439.6</v>
@@ -8486,7 +8486,7 @@
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="5" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="B328" s="4">
         <v>1439.3</v>
@@ -8506,7 +8506,7 @@
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="5" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="B329" s="4">
         <v>1438.3</v>
@@ -8526,7 +8526,7 @@
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="5" t="s">
-        <v>330</v>
+        <v>484</v>
       </c>
       <c r="B330" s="4">
         <v>1438.3</v>
@@ -8546,7 +8546,7 @@
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="5" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="B331" s="4">
         <v>1438.3</v>
@@ -8566,7 +8566,7 @@
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="5" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="B332" s="4">
         <v>1436.9</v>
@@ -8586,7 +8586,7 @@
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="5" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="B333" s="4">
         <v>1436.5</v>
@@ -8606,7 +8606,7 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="5" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="B334" s="4">
         <v>1436.4</v>
@@ -8626,7 +8626,7 @@
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="5" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="B335" s="4">
         <v>1435.5</v>
@@ -8646,7 +8646,7 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="5" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="B336" s="4">
         <v>1434.2</v>
@@ -8666,7 +8666,7 @@
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="5" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="B337" s="4">
         <v>1434.1</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="B338" s="4">
         <v>1433.2</v>
@@ -8706,7 +8706,7 @@
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="5" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="B339" s="4">
         <v>1432</v>
@@ -8726,7 +8726,7 @@
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="B340" s="4">
         <v>1431.8</v>
@@ -8746,7 +8746,7 @@
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="5" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="B341" s="4">
         <v>1430.7</v>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="5" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="B342" s="4">
         <v>1430.7</v>
@@ -8786,7 +8786,7 @@
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="5" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="B343" s="4">
         <v>1429.9</v>
@@ -8806,7 +8806,7 @@
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="5" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="B344" s="4">
         <v>1429.8</v>
@@ -8826,7 +8826,7 @@
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="B345" s="4">
         <v>1427.4</v>
@@ -8846,7 +8846,7 @@
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="5" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="B346" s="4">
         <v>1425.5</v>
@@ -8866,7 +8866,7 @@
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" s="5" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="B347" s="4">
         <v>1424.7</v>
@@ -8886,7 +8886,7 @@
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="B348" s="4">
         <v>1422.6</v>
@@ -8906,7 +8906,7 @@
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" s="5" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="B349" s="4">
         <v>1421.8</v>
@@ -8926,7 +8926,7 @@
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="5" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="B350" s="4">
         <v>1421.8</v>
@@ -8946,7 +8946,7 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="B351" s="4">
         <v>1420.6</v>
@@ -8966,7 +8966,7 @@
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="5" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="B352" s="4">
         <v>1420.3</v>
@@ -8986,7 +8986,7 @@
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="B353" s="4">
         <v>1420.2</v>
@@ -9006,7 +9006,7 @@
     </row>
     <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="5" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="B354" s="4">
         <v>1419.4</v>
@@ -9026,7 +9026,7 @@
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="5" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="B355" s="4">
         <v>1419</v>
@@ -9046,7 +9046,7 @@
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="B356" s="4">
         <v>1418.5</v>
@@ -9066,7 +9066,7 @@
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="5" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="B357" s="4">
         <v>1418.1</v>
@@ -9086,7 +9086,7 @@
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="B358" s="4">
         <v>1417.3</v>
@@ -9106,7 +9106,7 @@
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="5" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B359" s="4">
         <v>1414.6</v>
@@ -9126,7 +9126,7 @@
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="5" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="B360" s="4">
         <v>1413.6</v>
@@ -9146,7 +9146,7 @@
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="B361" s="4">
         <v>1413.6</v>
@@ -9166,7 +9166,7 @@
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="5" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="B362" s="4">
         <v>1412.7</v>
@@ -9186,7 +9186,7 @@
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="B363" s="4">
         <v>1412.3</v>
@@ -9204,9 +9204,9 @@
         <v>1421.2</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="21.6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
-        <v>364</v>
+        <v>485</v>
       </c>
       <c r="B364" s="4">
         <v>1412.1</v>
@@ -9226,7 +9226,7 @@
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="5" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="B365" s="4">
         <v>1411.9</v>
@@ -9246,7 +9246,7 @@
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="5" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="B366" s="4">
         <v>1411.3</v>
@@ -9266,7 +9266,7 @@
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="5" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="B367" s="4">
         <v>1410.9</v>
@@ -9286,7 +9286,7 @@
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="5" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="B368" s="4">
         <v>1410.2</v>
@@ -9306,7 +9306,7 @@
     </row>
     <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" s="5" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="B369" s="4">
         <v>1409.9</v>
@@ -9326,7 +9326,7 @@
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="B370" s="4">
         <v>1409.5</v>
@@ -9346,7 +9346,7 @@
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" s="5" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="B371" s="4">
         <v>1408.8</v>
@@ -9366,7 +9366,7 @@
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" s="5" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="B372" s="4">
         <v>1407.3</v>
@@ -9386,7 +9386,7 @@
     </row>
     <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" s="5" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="B373" s="4">
         <v>1406.1</v>
@@ -9406,7 +9406,7 @@
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" s="5" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="B374" s="4">
         <v>1400.2</v>
@@ -9426,7 +9426,7 @@
     </row>
     <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="B375" s="4">
         <v>1400.2</v>
@@ -9446,7 +9446,7 @@
     </row>
     <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" s="5" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="B376" s="4">
         <v>1399.6</v>
@@ -9466,7 +9466,7 @@
     </row>
     <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" s="5" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="B377" s="4">
         <v>1399</v>
@@ -9486,7 +9486,7 @@
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="B378" s="4">
         <v>1398.8</v>
@@ -9506,7 +9506,7 @@
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" s="5" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="B379" s="4">
         <v>1397.2</v>
@@ -9526,7 +9526,7 @@
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="5" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="B380" s="4">
         <v>1396.3</v>
@@ -9546,7 +9546,7 @@
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
-        <v>381</v>
+        <v>486</v>
       </c>
       <c r="B381" s="4">
         <v>1396.2</v>
@@ -9566,7 +9566,7 @@
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="5" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="B382" s="4">
         <v>1395.5</v>
@@ -9586,7 +9586,7 @@
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="5" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="B383" s="4">
         <v>1394.8</v>
@@ -9606,7 +9606,7 @@
     </row>
     <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="5" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="B384" s="4">
         <v>1393.8</v>
@@ -9626,7 +9626,7 @@
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" s="5" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B385" s="4">
         <v>1393.6</v>
@@ -9646,7 +9646,7 @@
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="B386" s="4">
         <v>1389.3</v>
@@ -9666,7 +9666,7 @@
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="B387" s="4">
         <v>1388.6</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="B388" s="4">
         <v>1386.8</v>
@@ -9706,7 +9706,7 @@
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="B389" s="4">
         <v>1385.7</v>
@@ -9726,7 +9726,7 @@
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="B390" s="4">
         <v>1385.6</v>
@@ -9746,7 +9746,7 @@
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="B391" s="4">
         <v>1384.9</v>
@@ -9766,7 +9766,7 @@
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="B392" s="4">
         <v>1384.5</v>
@@ -9786,7 +9786,7 @@
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="B393" s="4">
         <v>1384.2</v>
@@ -9806,7 +9806,7 @@
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B394" s="4">
         <v>1383</v>
@@ -9826,7 +9826,7 @@
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B395" s="4">
         <v>1382.9</v>
@@ -9846,7 +9846,7 @@
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" s="5" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="B396" s="4">
         <v>1379.7</v>
@@ -9866,7 +9866,7 @@
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" s="5" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="B397" s="4">
         <v>1379.6</v>
@@ -9886,7 +9886,7 @@
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" s="5" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="B398" s="4">
         <v>1378.7</v>
@@ -9906,7 +9906,7 @@
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="5" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="B399" s="4">
         <v>1376.7</v>
@@ -9926,7 +9926,7 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="5" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="B400" s="4">
         <v>1374.2</v>
@@ -9946,7 +9946,7 @@
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" s="5" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="B401" s="4">
         <v>1371.4</v>
@@ -9966,7 +9966,7 @@
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402" s="5" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="B402" s="4">
         <v>1369.7</v>
@@ -9986,7 +9986,7 @@
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" s="5" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="B403" s="4">
         <v>1367.5</v>
@@ -10006,7 +10006,7 @@
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404" s="5" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="B404" s="4">
         <v>1365.6</v>
@@ -10026,7 +10026,7 @@
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405" s="5" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="B405" s="4">
         <v>1365.1</v>
@@ -10046,7 +10046,7 @@
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" s="5" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="B406" s="4">
         <v>1363.4</v>
@@ -10066,7 +10066,7 @@
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" s="5" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="B407" s="4">
         <v>1361.1</v>
@@ -10086,7 +10086,7 @@
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408" s="5" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="B408" s="4">
         <v>1360.6</v>
@@ -10106,7 +10106,7 @@
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409" s="5" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="B409" s="4">
         <v>1360.3</v>
@@ -10126,7 +10126,7 @@
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410" s="5" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="B410" s="4">
         <v>1359.9</v>
@@ -10146,7 +10146,7 @@
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" s="5" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="B411" s="4">
         <v>1358.5</v>
@@ -10166,7 +10166,7 @@
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" s="5" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="B412" s="4">
         <v>1357.5</v>
@@ -10186,7 +10186,7 @@
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A413" s="5" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="B413" s="4">
         <v>1357.2</v>
@@ -10206,7 +10206,7 @@
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414" s="5" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="B414" s="4">
         <v>1356.2</v>
@@ -10226,7 +10226,7 @@
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A415" s="5" t="s">
-        <v>415</v>
+        <v>487</v>
       </c>
       <c r="B415" s="4">
         <v>1355.6</v>
@@ -10246,7 +10246,7 @@
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A416" s="5" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B416" s="4">
         <v>1353.3</v>
@@ -10266,7 +10266,7 @@
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A417" s="5" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="B417" s="4">
         <v>1351.5</v>
@@ -10286,7 +10286,7 @@
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418" s="5" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B418" s="4">
         <v>1351.4</v>
@@ -10306,7 +10306,7 @@
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419" s="5" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="B419" s="4">
         <v>1350.5</v>
@@ -10326,7 +10326,7 @@
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420" s="5" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="B420" s="4">
         <v>1346.7</v>
@@ -10346,7 +10346,7 @@
     </row>
     <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="B421" s="4">
         <v>1345.7</v>
@@ -10366,7 +10366,7 @@
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422" s="5" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="B422" s="4">
         <v>1344.1</v>
@@ -10386,7 +10386,7 @@
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423" s="5" t="s">
-        <v>423</v>
+        <v>488</v>
       </c>
       <c r="B423" s="4">
         <v>1343.7</v>
@@ -10406,7 +10406,7 @@
     </row>
     <row r="424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A424" s="5" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="B424" s="4">
         <v>1342.3</v>
@@ -10426,7 +10426,7 @@
     </row>
     <row r="425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A425" s="5" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="B425" s="4">
         <v>1338.6</v>
@@ -10446,7 +10446,7 @@
     </row>
     <row r="426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A426" s="5" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
       <c r="B426" s="4">
         <v>1337.9</v>
@@ -10466,7 +10466,7 @@
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427" s="5" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="B427" s="4">
         <v>1337.5</v>
@@ -10486,7 +10486,7 @@
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A428" s="5" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
       <c r="B428" s="4">
         <v>1337.1</v>
@@ -10506,7 +10506,7 @@
     </row>
     <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429" s="5" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="B429" s="4">
         <v>1334.1</v>
@@ -10526,7 +10526,7 @@
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430" s="5" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="B430" s="4">
         <v>1331.9</v>
@@ -10546,7 +10546,7 @@
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" s="5" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="B431" s="4">
         <v>1330.6</v>
@@ -10566,7 +10566,7 @@
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" s="5" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="B432" s="4">
         <v>1329.3</v>
@@ -10586,7 +10586,7 @@
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" s="5" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="B433" s="4">
         <v>1329.2</v>
@@ -10606,7 +10606,7 @@
     </row>
     <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" s="5" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
       <c r="B434" s="4">
         <v>1326.5</v>
@@ -10626,7 +10626,7 @@
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435" s="5" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="B435" s="4">
         <v>1324.4</v>
@@ -10646,7 +10646,7 @@
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436" s="5" t="s">
-        <v>436</v>
+        <v>489</v>
       </c>
       <c r="B436" s="4">
         <v>1324</v>
@@ -10666,7 +10666,7 @@
     </row>
     <row r="437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A437" s="5" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B437" s="4">
         <v>1323.8</v>
@@ -10686,7 +10686,7 @@
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" s="5" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="B438" s="4">
         <v>1321.3</v>
@@ -10706,7 +10706,7 @@
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439" s="5" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="B439" s="4">
         <v>1320.6</v>
@@ -10726,7 +10726,7 @@
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A440" s="5" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="B440" s="4">
         <v>1320.5</v>
@@ -10746,7 +10746,7 @@
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A441" s="5" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="B441" s="4">
         <v>1319.4</v>
@@ -10766,7 +10766,7 @@
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A442" s="5" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="B442" s="4">
         <v>1317.8</v>
@@ -10786,7 +10786,7 @@
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A443" s="5" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="B443" s="4">
         <v>1314.8</v>
@@ -10806,7 +10806,7 @@
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444" s="5" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="B444" s="4">
         <v>1312.1</v>
@@ -10826,7 +10826,7 @@
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A445" s="5" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="B445" s="4">
         <v>1310.5</v>
@@ -10846,7 +10846,7 @@
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446" s="5" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B446" s="4">
         <v>1309.2</v>
@@ -10866,7 +10866,7 @@
     </row>
     <row r="447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A447" s="5" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="B447" s="4">
         <v>1307.3</v>
@@ -10886,7 +10886,7 @@
     </row>
     <row r="448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A448" s="5" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="B448" s="4">
         <v>1305.2</v>
@@ -10906,7 +10906,7 @@
     </row>
     <row r="449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A449" s="5" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="B449" s="4">
         <v>1301.3</v>
@@ -10926,7 +10926,7 @@
     </row>
     <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450" s="5" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B450" s="4">
         <v>1301.0999999999999</v>
@@ -10946,7 +10946,7 @@
     </row>
     <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451" s="5" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="B451" s="4">
         <v>1301.0999999999999</v>
@@ -10966,7 +10966,7 @@
     </row>
     <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452" s="5" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="B452" s="4">
         <v>1300.7</v>
@@ -10986,7 +10986,7 @@
     </row>
     <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" s="5" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="B453" s="4">
         <v>1300.4000000000001</v>
@@ -11006,7 +11006,7 @@
     </row>
     <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" s="5" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
       <c r="B454" s="4">
         <v>1294.5999999999999</v>
@@ -11026,7 +11026,7 @@
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="5" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
       <c r="B455" s="4">
         <v>1292.5</v>
@@ -11046,7 +11046,7 @@
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" s="5" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="B456" s="4">
         <v>1292.0999999999999</v>
@@ -11066,7 +11066,7 @@
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457" s="5" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="B457" s="4">
         <v>1286.5999999999999</v>
@@ -11086,7 +11086,7 @@
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" s="5" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="B458" s="4">
         <v>1283.5</v>
@@ -11106,7 +11106,7 @@
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459" s="5" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="B459" s="4">
         <v>1283.2</v>
@@ -11126,7 +11126,7 @@
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" s="5" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="B460" s="4">
         <v>1282.4000000000001</v>
@@ -11146,7 +11146,7 @@
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461" s="5" t="s">
-        <v>461</v>
+        <v>490</v>
       </c>
       <c r="B461" s="4">
         <v>1282.0999999999999</v>
@@ -11166,7 +11166,7 @@
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462" s="5" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
       <c r="B462" s="4">
         <v>1276.5</v>
@@ -11186,7 +11186,7 @@
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463" s="5" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="B463" s="4">
         <v>1271.3</v>
@@ -11206,7 +11206,7 @@
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464" s="5" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
       <c r="B464" s="4">
         <v>1269.5999999999999</v>
@@ -11226,7 +11226,7 @@
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465" s="5" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
       <c r="B465" s="4">
         <v>1269.5</v>
@@ -11246,7 +11246,7 @@
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466" s="5" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="B466" s="4">
         <v>1265.2</v>
@@ -11266,7 +11266,7 @@
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467" s="5" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="B467" s="4">
         <v>1265.2</v>
@@ -11286,7 +11286,7 @@
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A468" s="5" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="B468" s="4">
         <v>1263.7</v>
@@ -11304,9 +11304,9 @@
         <v>1253.0999999999999</v>
       </c>
     </row>
-    <row r="469" spans="1:6" ht="21.6" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A469" s="5" t="s">
-        <v>469</v>
+        <v>491</v>
       </c>
       <c r="B469" s="4">
         <v>1261.4000000000001</v>
@@ -11326,7 +11326,7 @@
     </row>
     <row r="470" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A470" s="5" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="B470" s="4">
         <v>1257.5999999999999</v>
@@ -11346,7 +11346,7 @@
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A471" s="5" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="B471" s="4">
         <v>1251.9000000000001</v>
@@ -11366,7 +11366,7 @@
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A472" s="5" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="B472" s="4">
         <v>1250.5999999999999</v>
@@ -11386,7 +11386,7 @@
     </row>
     <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
-        <v>473</v>
+        <v>448</v>
       </c>
       <c r="B473" s="4">
         <v>1249.2</v>
@@ -11406,7 +11406,7 @@
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A474" s="5" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
       <c r="B474" s="4">
         <v>1225.5999999999999</v>
@@ -11426,7 +11426,7 @@
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A475" s="5" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="B475" s="4">
         <v>1221</v>
@@ -11446,7 +11446,7 @@
     </row>
     <row r="476" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A476" s="5" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="B476" s="4">
         <v>1220.7</v>
@@ -11466,7 +11466,7 @@
     </row>
     <row r="477" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A477" s="5" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="B477" s="4">
         <v>1217.0999999999999</v>
@@ -11486,7 +11486,7 @@
     </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478" s="5" t="s">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="B478" s="4">
         <v>1215.4000000000001</v>
@@ -11506,7 +11506,7 @@
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A479" s="5" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="B479" s="4">
         <v>1213.5</v>
@@ -11526,7 +11526,7 @@
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A480" s="5" t="s">
-        <v>480</v>
+        <v>455</v>
       </c>
       <c r="B480" s="4">
         <v>1210.8</v>
@@ -11546,7 +11546,7 @@
     </row>
     <row r="481" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A481" s="5" t="s">
-        <v>481</v>
+        <v>456</v>
       </c>
       <c r="B481" s="4">
         <v>1209.7</v>
@@ -11566,7 +11566,7 @@
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A482" s="5" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
       <c r="B482" s="4">
         <v>1201.4000000000001</v>
@@ -11586,7 +11586,7 @@
     </row>
     <row r="483" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A483" s="5" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="B483" s="4">
         <v>1199.5</v>
@@ -11606,7 +11606,7 @@
     </row>
     <row r="484" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A484" s="5" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
       <c r="B484" s="4">
         <v>1191.5</v>
@@ -11626,7 +11626,7 @@
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A485" s="5" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="B485" s="4">
         <v>1169.5</v>
@@ -11646,7 +11646,7 @@
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A486" s="5" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="B486" s="4">
         <v>1151.5</v>
@@ -11666,7 +11666,7 @@
     </row>
     <row r="487" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A487" s="5" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="B487" s="4">
         <v>1146.4000000000001</v>
@@ -11686,7 +11686,7 @@
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A488" s="5" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="B488" s="4">
         <v>1122.9000000000001</v>

</xml_diff>